<commit_message>
latest source with api
</commit_message>
<xml_diff>
--- a/API Details.xlsx
+++ b/API Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GCity\exportimport\SpreadJS\samples\gitGrapecity\Grape-City-Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD1D68C8-3231-4890-AAFC-6F80ED37B2A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFA62F9-85FC-4A0A-AF35-D1CCEB80898E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{48B28394-D047-4550-A9BE-DD2674A073ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{48B28394-D047-4550-A9BE-DD2674A073ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -645,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69DD561-DBAA-4917-8E91-BEC80B17B129}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -797,11 +797,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441D3FFE-5E59-4128-8F82-C33970D30F62}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>